<commit_message>
PGS update to docs
</commit_message>
<xml_diff>
--- a/documents/Deliverable_3/FlyingMongeese_Deliverable_3_ProductBacklog.xlsx
+++ b/documents/Deliverable_3/FlyingMongeese_Deliverable_3_ProductBacklog.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aaron\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A13292F-FA9A-4935-8C13-FFCB5F42B2B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2B677B-A59D-451A-BD85-D32B799500A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12705" yWindow="435" windowWidth="12900" windowHeight="15555" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -60,9 +60,6 @@
     <t>As a small business owner,I want to be able to input the total revenue made for the day into the database upon closing so that I can use that data to update the accuracy of the software</t>
   </si>
   <si>
-    <t>As a small business owner,I want to use my sales report from past years so that I can get an estimate prediction of future sales</t>
-  </si>
-  <si>
     <t>As a small business owner,I want to use sales report from past years so that I can see requirements needed to hit specific sales margins</t>
   </si>
   <si>
@@ -94,13 +91,16 @@
   </si>
   <si>
     <t>4,5</t>
+  </si>
+  <si>
+    <t>As a small business owner,I want to use my sales reports from past years so that I can get an estimate prediction of future sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -113,6 +113,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -129,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,30 +143,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +495,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -500,282 +526,285 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="7">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="10">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="10">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>16</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>17</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10">
         <v>8</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="10">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>18</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="6">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1">
-        <v>8</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="10">
         <v>6</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10">
         <v>10</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>16</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>17</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>18</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>19</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>20</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="1">
+        <f>SUM(F2:F12)</f>
         <v>48</v>
       </c>
     </row>
@@ -796,5 +825,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Touches before Submission of documents
</commit_message>
<xml_diff>
--- a/documents/Deliverable_3/FlyingMongeese_Deliverable_3_ProductBacklog.xlsx
+++ b/documents/Deliverable_3/FlyingMongeese_Deliverable_3_ProductBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Bhakta\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1DFFE7-6294-4C6B-A707-D629DC5741F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD4F074-42F7-45D0-8FBF-F1A4BB9A234D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="435" windowWidth="12900" windowHeight="15555" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12708" yWindow="432" windowWidth="12900" windowHeight="15552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,21 +182,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,265 +511,265 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <v>8</v>
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>8</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+    <row r="4" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>6</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row r="5" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>13</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>4</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    <row r="6" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row r="7" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>15</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>5</v>
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    <row r="8" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>2</v>
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+    <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>17</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>8</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>2</v>
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    <row r="10" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>18</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>9</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>2</v>
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+    <row r="11" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>19</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
         <v>11</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>6</v>
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>20</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="8">
         <v>10</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -773,7 +779,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="6"/>
       <c r="C14" s="3"/>
@@ -781,7 +787,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="6"/>
       <c r="C15" s="3"/>
@@ -789,7 +795,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="6"/>
       <c r="C16" s="3"/>
@@ -797,7 +803,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="6"/>
       <c r="C17" s="3"/>
@@ -805,7 +811,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>